<commit_message>
Display All Courses on StudentDashboard
</commit_message>
<xml_diff>
--- a/Enrollment exmaple data for Lab8.xlsx
+++ b/Enrollment exmaple data for Lab8.xlsx
@@ -96,7 +96,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +106,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -145,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -162,10 +168,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -485,12 +488,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -513,7 +516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -533,7 +536,7 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -545,7 +548,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -557,7 +560,7 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -575,9 +578,9 @@
       <c r="C6" s="3"/>
       <c r="D6" s="6"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="F6" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -597,7 +600,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -609,7 +612,7 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -621,7 +624,7 @@
         <v>94</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -633,7 +636,7 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -651,7 +654,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="6"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="7"/>
+      <c r="F12" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="3"/>
@@ -659,9 +662,9 @@
       <c r="C13" s="3"/>
       <c r="D13" s="6"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+      <c r="F13" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
@@ -681,7 +684,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -693,7 +696,7 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -705,7 +708,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -723,7 +726,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="6"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="7"/>
+      <c r="F18" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="3" t="s">

</xml_diff>

<commit_message>
Added Students Enrolled For Student Dash
</commit_message>
<xml_diff>
--- a/Enrollment exmaple data for Lab8.xlsx
+++ b/Enrollment exmaple data for Lab8.xlsx
@@ -96,7 +96,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,12 +114,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -151,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -168,13 +162,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -488,12 +476,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -540,7 +528,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="6"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
@@ -552,7 +540,7 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="6"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
@@ -564,7 +552,7 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="6"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
@@ -572,13 +560,13 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="6"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
@@ -604,7 +592,7 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="6"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
@@ -616,7 +604,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="3" t="s">
         <v>17</v>
       </c>
@@ -628,7 +616,7 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="6"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
@@ -640,7 +628,7 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="6"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
@@ -648,21 +636,21 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="6"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
@@ -688,7 +676,7 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="6"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="3" t="s">
         <v>22</v>
       </c>
@@ -700,7 +688,7 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="6"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="3" t="s">
         <v>16</v>
       </c>
@@ -712,7 +700,7 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="6"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="3" t="s">
         <v>17</v>
       </c>
@@ -724,9 +712,9 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="6"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="6"/>
+      <c r="F18" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="3" t="s">
@@ -752,7 +740,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="3" t="s">
         <v>16</v>
       </c>
@@ -764,7 +752,7 @@
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="6"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="3" t="s">
         <v>22</v>
       </c>
@@ -776,7 +764,7 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="6"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="3" t="s">
         <v>11</v>
       </c>

</xml_diff>